<commit_message>
Temperature Analyzer Rev 1
</commit_message>
<xml_diff>
--- a/Python Heat Transfer Analysis/solarData.xlsx
+++ b/Python Heat Transfer Analysis/solarData.xlsx
@@ -1,37 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtran\Desktop\solarModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtran\Documents\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8ADDC2-9B7B-4ABC-BF0C-541704BC4360}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1489A8-E176-4424-9FC8-54F82ECD337A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="2580" windowWidth="16920" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="121">
   <si>
     <t>Testing Date</t>
   </si>
@@ -94,292 +84,277 @@
     <t>12-01-2019</t>
   </si>
   <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Temp1 [C]</t>
+  </si>
+  <si>
+    <t>Temp2 [C]</t>
+  </si>
+  <si>
+    <t>Temp_a [C]</t>
+  </si>
+  <si>
+    <t>16:32:00</t>
+  </si>
+  <si>
+    <t>16:37:00</t>
+  </si>
+  <si>
+    <t>16:42:00</t>
+  </si>
+  <si>
+    <t>16:47:00</t>
+  </si>
+  <si>
+    <t>16:52:00</t>
+  </si>
+  <si>
+    <t>16:57:00</t>
+  </si>
+  <si>
+    <t>17:02:00</t>
+  </si>
+  <si>
+    <t>17:07:00</t>
+  </si>
+  <si>
+    <t>17:12:00</t>
+  </si>
+  <si>
+    <t>17:17:00</t>
+  </si>
+  <si>
+    <t>17:22:00</t>
+  </si>
+  <si>
+    <t>17:27:00</t>
+  </si>
+  <si>
+    <t>17:32:00</t>
+  </si>
+  <si>
+    <t>17:37:00</t>
+  </si>
+  <si>
+    <t>17:42:00</t>
+  </si>
+  <si>
+    <t>17:47:00</t>
+  </si>
+  <si>
+    <t>17:52:00</t>
+  </si>
+  <si>
+    <t>17:57:00</t>
+  </si>
+  <si>
+    <t>08:50:00</t>
+  </si>
+  <si>
+    <t>08:55:00</t>
+  </si>
+  <si>
+    <t>09:00:00</t>
+  </si>
+  <si>
+    <t>09:05:00</t>
+  </si>
+  <si>
+    <t>09:10:00</t>
+  </si>
+  <si>
+    <t>09:15:00</t>
+  </si>
+  <si>
+    <t>09:20:00</t>
+  </si>
+  <si>
+    <t>09:25:00</t>
+  </si>
+  <si>
+    <t>09:30:00</t>
+  </si>
+  <si>
+    <t>09:35:00</t>
+  </si>
+  <si>
+    <t>09:40:00</t>
+  </si>
+  <si>
+    <t>09:45:00</t>
+  </si>
+  <si>
+    <t>09:50:00</t>
+  </si>
+  <si>
+    <t>09:55:00</t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t>10:05:00</t>
+  </si>
+  <si>
+    <t>10:10:00</t>
+  </si>
+  <si>
+    <t>10:15:00</t>
+  </si>
+  <si>
+    <t>10:20:00</t>
+  </si>
+  <si>
+    <t>10:25:00</t>
+  </si>
+  <si>
+    <t>10:30:00</t>
+  </si>
+  <si>
+    <t>10:35:00</t>
+  </si>
+  <si>
+    <t>10:40:00</t>
+  </si>
+  <si>
+    <t>10:45:00</t>
+  </si>
+  <si>
+    <t>10:50:00</t>
+  </si>
+  <si>
+    <t>10:55:00</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
+  </si>
+  <si>
+    <t>11:05:00</t>
+  </si>
+  <si>
+    <t>11:10:00</t>
+  </si>
+  <si>
+    <t>11:15:00</t>
+  </si>
+  <si>
+    <t>11:20:00</t>
+  </si>
+  <si>
+    <t>11:25:00</t>
+  </si>
+  <si>
+    <t>11:30:00</t>
+  </si>
+  <si>
+    <t>11:35:00</t>
+  </si>
+  <si>
+    <t>11:40:00</t>
+  </si>
+  <si>
+    <t>11:45:00</t>
+  </si>
+  <si>
+    <t>11:50:00</t>
+  </si>
+  <si>
+    <t>11:55:00</t>
+  </si>
+  <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t>12:05:00</t>
+  </si>
+  <si>
+    <t>12:10:00</t>
+  </si>
+  <si>
+    <t>12:15:00</t>
+  </si>
+  <si>
+    <t>12:20:00</t>
+  </si>
+  <si>
+    <t>12:25:00</t>
+  </si>
+  <si>
+    <t>12:30:00</t>
+  </si>
+  <si>
+    <t>12:35:00</t>
+  </si>
+  <si>
+    <t>12:40:00</t>
+  </si>
+  <si>
+    <t>12:45:00</t>
+  </si>
+  <si>
+    <t>12:50:00</t>
+  </si>
+  <si>
+    <t>12:55:00</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>13:05:00</t>
+  </si>
+  <si>
+    <t>13:10:00</t>
+  </si>
+  <si>
+    <t>13:15:00</t>
+  </si>
+  <si>
+    <t>13:20:00</t>
+  </si>
+  <si>
+    <t>13:25:00</t>
+  </si>
+  <si>
+    <t>13:30:00</t>
+  </si>
+  <si>
+    <t>13:35:00</t>
+  </si>
+  <si>
+    <t>13:40:00</t>
+  </si>
+  <si>
+    <t>13:45:00</t>
+  </si>
+  <si>
+    <t>13:50:00</t>
+  </si>
+  <si>
+    <t>13:55:00</t>
+  </si>
+  <si>
+    <t>14:00:00</t>
+  </si>
+  <si>
+    <t>14:05:00</t>
+  </si>
+  <si>
+    <t>14:10:00</t>
+  </si>
+  <si>
+    <t>14:15:00</t>
+  </si>
+  <si>
     <t>Test</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Light Drizzle</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Cloudy</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Temp1 [C]</t>
-  </si>
-  <si>
-    <t>Temp2 [C]</t>
-  </si>
-  <si>
-    <t>Temp_a [C]</t>
-  </si>
-  <si>
-    <t>16:32:00</t>
-  </si>
-  <si>
-    <t>16:37:00</t>
-  </si>
-  <si>
-    <t>16:42:00</t>
-  </si>
-  <si>
-    <t>16:47:00</t>
-  </si>
-  <si>
-    <t>16:52:00</t>
-  </si>
-  <si>
-    <t>16:57:00</t>
-  </si>
-  <si>
-    <t>17:02:00</t>
-  </si>
-  <si>
-    <t>17:07:00</t>
-  </si>
-  <si>
-    <t>17:12:00</t>
-  </si>
-  <si>
-    <t>17:17:00</t>
-  </si>
-  <si>
-    <t>17:22:00</t>
-  </si>
-  <si>
-    <t>17:27:00</t>
-  </si>
-  <si>
-    <t>17:32:00</t>
-  </si>
-  <si>
-    <t>17:37:00</t>
-  </si>
-  <si>
-    <t>17:42:00</t>
-  </si>
-  <si>
-    <t>17:47:00</t>
-  </si>
-  <si>
-    <t>17:52:00</t>
-  </si>
-  <si>
-    <t>17:57:00</t>
-  </si>
-  <si>
-    <t>08:50:00</t>
-  </si>
-  <si>
-    <t>08:55:00</t>
-  </si>
-  <si>
-    <t>09:00:00</t>
-  </si>
-  <si>
-    <t>09:05:00</t>
-  </si>
-  <si>
-    <t>09:10:00</t>
-  </si>
-  <si>
-    <t>09:15:00</t>
-  </si>
-  <si>
-    <t>09:20:00</t>
-  </si>
-  <si>
-    <t>09:25:00</t>
-  </si>
-  <si>
-    <t>09:30:00</t>
-  </si>
-  <si>
-    <t>09:35:00</t>
-  </si>
-  <si>
-    <t>09:40:00</t>
-  </si>
-  <si>
-    <t>09:45:00</t>
-  </si>
-  <si>
-    <t>09:50:00</t>
-  </si>
-  <si>
-    <t>09:55:00</t>
-  </si>
-  <si>
-    <t>10:00:00</t>
-  </si>
-  <si>
-    <t>10:05:00</t>
-  </si>
-  <si>
-    <t>10:10:00</t>
-  </si>
-  <si>
-    <t>10:15:00</t>
-  </si>
-  <si>
-    <t>10:20:00</t>
-  </si>
-  <si>
-    <t>10:25:00</t>
-  </si>
-  <si>
-    <t>10:30:00</t>
-  </si>
-  <si>
-    <t>10:35:00</t>
-  </si>
-  <si>
-    <t>10:40:00</t>
-  </si>
-  <si>
-    <t>10:45:00</t>
-  </si>
-  <si>
-    <t>10:50:00</t>
-  </si>
-  <si>
-    <t>10:55:00</t>
-  </si>
-  <si>
-    <t>11:00:00</t>
-  </si>
-  <si>
-    <t>11:05:00</t>
-  </si>
-  <si>
-    <t>11:10:00</t>
-  </si>
-  <si>
-    <t>11:15:00</t>
-  </si>
-  <si>
-    <t>11:20:00</t>
-  </si>
-  <si>
-    <t>11:25:00</t>
-  </si>
-  <si>
-    <t>11:30:00</t>
-  </si>
-  <si>
-    <t>11:35:00</t>
-  </si>
-  <si>
-    <t>11:40:00</t>
-  </si>
-  <si>
-    <t>11:45:00</t>
-  </si>
-  <si>
-    <t>11:50:00</t>
-  </si>
-  <si>
-    <t>11:55:00</t>
-  </si>
-  <si>
-    <t>12:00:00</t>
-  </si>
-  <si>
-    <t>12:05:00</t>
-  </si>
-  <si>
-    <t>12:10:00</t>
-  </si>
-  <si>
-    <t>12:15:00</t>
-  </si>
-  <si>
-    <t>12:20:00</t>
-  </si>
-  <si>
-    <t>12:25:00</t>
-  </si>
-  <si>
-    <t>12:30:00</t>
-  </si>
-  <si>
-    <t>12:35:00</t>
-  </si>
-  <si>
-    <t>12:40:00</t>
-  </si>
-  <si>
-    <t>12:45:00</t>
-  </si>
-  <si>
-    <t>12:50:00</t>
-  </si>
-  <si>
-    <t>12:55:00</t>
-  </si>
-  <si>
-    <t>13:00:00</t>
-  </si>
-  <si>
-    <t>13:05:00</t>
-  </si>
-  <si>
-    <t>13:10:00</t>
-  </si>
-  <si>
-    <t>13:15:00</t>
-  </si>
-  <si>
-    <t>13:20:00</t>
-  </si>
-  <si>
-    <t>13:25:00</t>
-  </si>
-  <si>
-    <t>13:30:00</t>
-  </si>
-  <si>
-    <t>13:35:00</t>
-  </si>
-  <si>
-    <t>13:40:00</t>
-  </si>
-  <si>
-    <t>13:45:00</t>
-  </si>
-  <si>
-    <t>13:50:00</t>
-  </si>
-  <si>
-    <t>13:55:00</t>
-  </si>
-  <si>
-    <t>14:00:00</t>
-  </si>
-  <si>
-    <t>14:05:00</t>
-  </si>
-  <si>
-    <t>14:10:00</t>
-  </si>
-  <si>
-    <t>14:15:00</t>
   </si>
   <si>
     <t xml:space="preserve"> 10-03-2020</t>
@@ -416,8 +391,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -489,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -499,10 +475,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,17 +795,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.36328125" style="4" customWidth="1"/>
     <col min="2" max="2" width="16.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.36328125" style="4" customWidth="1"/>
     <col min="10" max="10" width="9.08984375" style="4" customWidth="1"/>
     <col min="11" max="11" width="18.36328125" style="4" customWidth="1"/>
@@ -848,7 +826,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -893,7 +871,7 @@
       <c r="C2">
         <v>0.1</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>43864.692361111112</v>
       </c>
       <c r="F2">
@@ -937,7 +915,7 @@
       <c r="C3">
         <v>0.1</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>43864.371527777781</v>
       </c>
       <c r="F3">
@@ -972,187 +950,50 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="6">
-        <v>43884.0476851852</v>
-      </c>
-      <c r="F4">
-        <v>3.806</v>
-      </c>
-      <c r="G4">
-        <v>26</v>
-      </c>
-      <c r="H4">
-        <v>85</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4">
-        <v>24.5</v>
-      </c>
-      <c r="K4">
-        <v>24</v>
-      </c>
-      <c r="L4">
-        <v>0.5</v>
-      </c>
-      <c r="M4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4">
-        <v>3.7829999999999999</v>
-      </c>
-      <c r="O4">
-        <v>10.46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="6">
-        <v>43885.0476851852</v>
-      </c>
-      <c r="F5">
-        <v>3.806</v>
-      </c>
-      <c r="G5">
-        <v>26</v>
-      </c>
-      <c r="H5">
-        <v>85</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5">
-        <v>24.5</v>
-      </c>
-      <c r="K5">
-        <v>24</v>
-      </c>
-      <c r="L5">
-        <v>0.5</v>
-      </c>
-      <c r="M5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5">
-        <v>3.7829999999999999</v>
-      </c>
-      <c r="O5">
-        <v>4.1840000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="6">
-        <v>43885.0476851852</v>
-      </c>
-      <c r="F6">
-        <v>3.806</v>
-      </c>
-      <c r="G6">
-        <v>26</v>
-      </c>
-      <c r="H6">
-        <v>85</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
-      </c>
-      <c r="K6">
-        <v>24</v>
-      </c>
-      <c r="L6">
-        <v>0.5</v>
-      </c>
-      <c r="M6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6">
-        <v>3.7829999999999999</v>
-      </c>
-      <c r="O6">
-        <v>6.2759999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="6">
-        <v>43885.0476851852</v>
-      </c>
-      <c r="F7">
-        <v>3.806</v>
-      </c>
-      <c r="G7">
-        <v>26</v>
-      </c>
-      <c r="H7">
-        <v>85</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7">
-        <v>24.5</v>
-      </c>
-      <c r="K7">
-        <v>24</v>
-      </c>
-      <c r="L7">
-        <v>0.5</v>
-      </c>
-      <c r="M7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7">
-        <v>3.7829999999999999</v>
-      </c>
-      <c r="O7">
-        <v>12.552</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="E4" s="8"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="O4"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -1168,19 +1009,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1188,7 +1029,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>21.9</v>
@@ -1205,7 +1046,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>22.1</v>
@@ -1222,7 +1063,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>22.8</v>
@@ -1239,7 +1080,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>22.9</v>
@@ -1256,7 +1097,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>23</v>
@@ -1273,7 +1114,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>23</v>
@@ -1290,7 +1131,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>23.1</v>
@@ -1307,7 +1148,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>23.1</v>
@@ -1324,7 +1165,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>23.1</v>
@@ -1341,7 +1182,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>23.1</v>
@@ -1358,7 +1199,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>23.1</v>
@@ -1375,7 +1216,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>23</v>
@@ -1392,7 +1233,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>23</v>
@@ -1409,7 +1250,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>23</v>
@@ -1426,7 +1267,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>22.9</v>
@@ -1443,7 +1284,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C17">
         <v>22.9</v>
@@ -1460,7 +1301,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>22.9</v>
@@ -1477,7 +1318,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>22.8</v>
@@ -1494,7 +1335,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>15.3</v>
@@ -1511,7 +1352,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>15</v>
@@ -1528,7 +1369,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>14.7</v>
@@ -1545,7 +1386,7 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C23">
         <v>14.3</v>
@@ -1562,7 +1403,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C24">
         <v>14</v>
@@ -1579,7 +1420,7 @@
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C25">
         <v>13.9</v>
@@ -1596,7 +1437,7 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C26">
         <v>14</v>
@@ -1613,7 +1454,7 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C27">
         <v>14.3</v>
@@ -1630,7 +1471,7 @@
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C28">
         <v>14.8</v>
@@ -1647,7 +1488,7 @@
         <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C29">
         <v>15.2</v>
@@ -1664,7 +1505,7 @@
         <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C30">
         <v>15.8</v>
@@ -1681,7 +1522,7 @@
         <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C31">
         <v>16.100000000000001</v>
@@ -1698,7 +1539,7 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C32">
         <v>16.600000000000001</v>
@@ -1715,7 +1556,7 @@
         <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C33">
         <v>17</v>
@@ -1732,7 +1573,7 @@
         <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C34">
         <v>17.600000000000001</v>
@@ -1749,7 +1590,7 @@
         <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C35">
         <v>18</v>
@@ -1766,7 +1607,7 @@
         <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C36">
         <v>18.5</v>
@@ -1783,7 +1624,7 @@
         <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C37">
         <v>18.899999999999999</v>
@@ -1800,7 +1641,7 @@
         <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C38">
         <v>19.8</v>
@@ -1817,7 +1658,7 @@
         <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C39">
         <v>19.899999999999999</v>
@@ -1834,7 +1675,7 @@
         <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C40">
         <v>20.2</v>
@@ -1851,7 +1692,7 @@
         <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C41">
         <v>20.6</v>
@@ -1868,7 +1709,7 @@
         <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C42">
         <v>21</v>
@@ -1885,7 +1726,7 @@
         <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C43">
         <v>21.4</v>
@@ -1902,7 +1743,7 @@
         <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C44">
         <v>21.9</v>
@@ -1919,7 +1760,7 @@
         <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C45">
         <v>22.4</v>
@@ -1936,7 +1777,7 @@
         <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C46">
         <v>22.7</v>
@@ -1953,7 +1794,7 @@
         <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C47">
         <v>23.2</v>
@@ -1970,7 +1811,7 @@
         <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C48">
         <v>23.7</v>
@@ -1987,7 +1828,7 @@
         <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C49">
         <v>24</v>
@@ -2004,7 +1845,7 @@
         <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C50">
         <v>24.3</v>
@@ -2021,7 +1862,7 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C51">
         <v>24.6</v>
@@ -2038,7 +1879,7 @@
         <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C52">
         <v>24.9</v>
@@ -2055,7 +1896,7 @@
         <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C53">
         <v>25.3</v>
@@ -2072,7 +1913,7 @@
         <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C54">
         <v>25.6</v>
@@ -2089,7 +1930,7 @@
         <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C55">
         <v>26</v>
@@ -2106,7 +1947,7 @@
         <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C56">
         <v>26.4</v>
@@ -2123,7 +1964,7 @@
         <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C57">
         <v>26.8</v>
@@ -2140,7 +1981,7 @@
         <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C58">
         <v>27.1</v>
@@ -2157,7 +1998,7 @@
         <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C59">
         <v>27.4</v>
@@ -2174,7 +2015,7 @@
         <v>19</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C60">
         <v>27.8</v>
@@ -2191,7 +2032,7 @@
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C61">
         <v>28.1</v>
@@ -2208,7 +2049,7 @@
         <v>19</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C62">
         <v>28.4</v>
@@ -2225,7 +2066,7 @@
         <v>19</v>
       </c>
       <c r="B63" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C63">
         <v>28.7</v>
@@ -2242,7 +2083,7 @@
         <v>19</v>
       </c>
       <c r="B64" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C64">
         <v>29</v>
@@ -2259,7 +2100,7 @@
         <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C65">
         <v>29.3</v>
@@ -2276,7 +2117,7 @@
         <v>19</v>
       </c>
       <c r="B66" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C66">
         <v>29.6</v>
@@ -2293,7 +2134,7 @@
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C67">
         <v>29.8</v>
@@ -2310,7 +2151,7 @@
         <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C68">
         <v>30.1</v>
@@ -2327,7 +2168,7 @@
         <v>19</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C69">
         <v>30.3</v>
@@ -2344,7 +2185,7 @@
         <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C70">
         <v>30.4</v>
@@ -2361,7 +2202,7 @@
         <v>19</v>
       </c>
       <c r="B71" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C71">
         <v>30.4</v>
@@ -2378,7 +2219,7 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C72">
         <v>30.4</v>
@@ -2395,7 +2236,7 @@
         <v>19</v>
       </c>
       <c r="B73" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C73">
         <v>30.9</v>
@@ -2412,7 +2253,7 @@
         <v>19</v>
       </c>
       <c r="B74" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C74">
         <v>31.4</v>
@@ -2429,7 +2270,7 @@
         <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C75">
         <v>31.6</v>
@@ -2446,7 +2287,7 @@
         <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C76">
         <v>31.8</v>
@@ -2463,7 +2304,7 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C77">
         <v>32</v>
@@ -2480,7 +2321,7 @@
         <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C78">
         <v>32.1</v>
@@ -2497,7 +2338,7 @@
         <v>19</v>
       </c>
       <c r="B79" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C79">
         <v>32.200000000000003</v>
@@ -2514,7 +2355,7 @@
         <v>19</v>
       </c>
       <c r="B80" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C80">
         <v>32.299999999999997</v>
@@ -2531,7 +2372,7 @@
         <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C81">
         <v>32.4</v>
@@ -2548,7 +2389,7 @@
         <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C82">
         <v>32.4</v>
@@ -2565,7 +2406,7 @@
         <v>19</v>
       </c>
       <c r="B83" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C83">
         <v>32.5</v>
@@ -2582,7 +2423,7 @@
         <v>19</v>
       </c>
       <c r="B84" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C84">
         <v>32.5</v>
@@ -2599,7 +2440,7 @@
         <v>19</v>
       </c>
       <c r="B85" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C85">
         <v>32.6</v>
@@ -2616,7 +2457,7 @@
         <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C86">
         <v>15.3</v>
@@ -2633,7 +2474,7 @@
         <v>19</v>
       </c>
       <c r="B87" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C87">
         <v>15</v>
@@ -2650,7 +2491,7 @@
         <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C88">
         <v>14.7</v>
@@ -2667,7 +2508,7 @@
         <v>19</v>
       </c>
       <c r="B89" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C89">
         <v>14.3</v>
@@ -2684,7 +2525,7 @@
         <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C90">
         <v>14</v>
@@ -2701,7 +2542,7 @@
         <v>19</v>
       </c>
       <c r="B91" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C91">
         <v>13.9</v>
@@ -2718,7 +2559,7 @@
         <v>19</v>
       </c>
       <c r="B92" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C92">
         <v>14</v>
@@ -2735,7 +2576,7 @@
         <v>19</v>
       </c>
       <c r="B93" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C93">
         <v>14.3</v>
@@ -2752,7 +2593,7 @@
         <v>19</v>
       </c>
       <c r="B94" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C94">
         <v>14.8</v>
@@ -2769,7 +2610,7 @@
         <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C95">
         <v>15.2</v>
@@ -2786,7 +2627,7 @@
         <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C96">
         <v>15.8</v>
@@ -2803,7 +2644,7 @@
         <v>19</v>
       </c>
       <c r="B97" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C97">
         <v>16.100000000000001</v>
@@ -2820,7 +2661,7 @@
         <v>19</v>
       </c>
       <c r="B98" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C98">
         <v>16.600000000000001</v>
@@ -2837,7 +2678,7 @@
         <v>19</v>
       </c>
       <c r="B99" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C99">
         <v>17</v>
@@ -2854,7 +2695,7 @@
         <v>19</v>
       </c>
       <c r="B100" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C100">
         <v>17.600000000000001</v>
@@ -2871,7 +2712,7 @@
         <v>19</v>
       </c>
       <c r="B101" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C101">
         <v>18</v>
@@ -2888,7 +2729,7 @@
         <v>19</v>
       </c>
       <c r="B102" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C102">
         <v>18.5</v>
@@ -2905,7 +2746,7 @@
         <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C103">
         <v>18.899999999999999</v>
@@ -2922,7 +2763,7 @@
         <v>19</v>
       </c>
       <c r="B104" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C104">
         <v>19.8</v>
@@ -2939,7 +2780,7 @@
         <v>19</v>
       </c>
       <c r="B105" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C105">
         <v>19.899999999999999</v>
@@ -2956,7 +2797,7 @@
         <v>19</v>
       </c>
       <c r="B106" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C106">
         <v>20.2</v>
@@ -2973,7 +2814,7 @@
         <v>19</v>
       </c>
       <c r="B107" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C107">
         <v>20.6</v>
@@ -2990,7 +2831,7 @@
         <v>19</v>
       </c>
       <c r="B108" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C108">
         <v>21</v>
@@ -3007,7 +2848,7 @@
         <v>19</v>
       </c>
       <c r="B109" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C109">
         <v>21.4</v>
@@ -3024,7 +2865,7 @@
         <v>19</v>
       </c>
       <c r="B110" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C110">
         <v>21.9</v>
@@ -3041,7 +2882,7 @@
         <v>19</v>
       </c>
       <c r="B111" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C111">
         <v>22.4</v>
@@ -3058,7 +2899,7 @@
         <v>19</v>
       </c>
       <c r="B112" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C112">
         <v>22.7</v>
@@ -3075,7 +2916,7 @@
         <v>19</v>
       </c>
       <c r="B113" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C113">
         <v>23.2</v>
@@ -3092,7 +2933,7 @@
         <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C114">
         <v>23.7</v>
@@ -3109,7 +2950,7 @@
         <v>19</v>
       </c>
       <c r="B115" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C115">
         <v>24</v>
@@ -3126,7 +2967,7 @@
         <v>19</v>
       </c>
       <c r="B116" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C116">
         <v>24.3</v>
@@ -3143,7 +2984,7 @@
         <v>19</v>
       </c>
       <c r="B117" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C117">
         <v>24.6</v>
@@ -3160,7 +3001,7 @@
         <v>19</v>
       </c>
       <c r="B118" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C118">
         <v>24.9</v>
@@ -3177,7 +3018,7 @@
         <v>19</v>
       </c>
       <c r="B119" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C119">
         <v>25.3</v>
@@ -3194,7 +3035,7 @@
         <v>19</v>
       </c>
       <c r="B120" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C120">
         <v>25.6</v>
@@ -3211,7 +3052,7 @@
         <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C121">
         <v>26</v>
@@ -3228,7 +3069,7 @@
         <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C122">
         <v>26.4</v>
@@ -3245,7 +3086,7 @@
         <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C123">
         <v>26.8</v>
@@ -3262,7 +3103,7 @@
         <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C124">
         <v>27.1</v>
@@ -3279,7 +3120,7 @@
         <v>19</v>
       </c>
       <c r="B125" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C125">
         <v>27.4</v>
@@ -3296,7 +3137,7 @@
         <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C126">
         <v>27.8</v>
@@ -3313,7 +3154,7 @@
         <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C127">
         <v>28.1</v>
@@ -3330,7 +3171,7 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C128">
         <v>28.4</v>
@@ -3347,7 +3188,7 @@
         <v>19</v>
       </c>
       <c r="B129" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C129">
         <v>28.7</v>
@@ -3364,7 +3205,7 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C130">
         <v>29</v>
@@ -3381,7 +3222,7 @@
         <v>19</v>
       </c>
       <c r="B131" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C131">
         <v>29.3</v>
@@ -3398,7 +3239,7 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C132">
         <v>29.6</v>
@@ -3415,7 +3256,7 @@
         <v>19</v>
       </c>
       <c r="B133" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C133">
         <v>29.8</v>
@@ -3432,7 +3273,7 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C134">
         <v>30.1</v>
@@ -3449,7 +3290,7 @@
         <v>19</v>
       </c>
       <c r="B135" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C135">
         <v>30.3</v>
@@ -3466,7 +3307,7 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C136">
         <v>30.4</v>
@@ -3483,7 +3324,7 @@
         <v>19</v>
       </c>
       <c r="B137" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C137">
         <v>30.4</v>
@@ -3500,7 +3341,7 @@
         <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C138">
         <v>30.4</v>
@@ -3517,7 +3358,7 @@
         <v>19</v>
       </c>
       <c r="B139" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C139">
         <v>30.9</v>
@@ -3534,7 +3375,7 @@
         <v>19</v>
       </c>
       <c r="B140" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C140">
         <v>31.4</v>
@@ -3551,7 +3392,7 @@
         <v>19</v>
       </c>
       <c r="B141" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C141">
         <v>31.6</v>
@@ -3568,7 +3409,7 @@
         <v>19</v>
       </c>
       <c r="B142" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C142">
         <v>31.8</v>
@@ -3585,7 +3426,7 @@
         <v>19</v>
       </c>
       <c r="B143" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C143">
         <v>32</v>
@@ -3602,7 +3443,7 @@
         <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C144">
         <v>32.1</v>
@@ -3619,7 +3460,7 @@
         <v>19</v>
       </c>
       <c r="B145" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C145">
         <v>32.200000000000003</v>
@@ -3636,7 +3477,7 @@
         <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C146">
         <v>32.299999999999997</v>
@@ -3653,7 +3494,7 @@
         <v>19</v>
       </c>
       <c r="B147" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C147">
         <v>32.4</v>
@@ -3670,7 +3511,7 @@
         <v>19</v>
       </c>
       <c r="B148" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C148">
         <v>32.4</v>
@@ -3687,7 +3528,7 @@
         <v>19</v>
       </c>
       <c r="B149" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C149">
         <v>32.5</v>
@@ -3704,7 +3545,7 @@
         <v>19</v>
       </c>
       <c r="B150" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C150">
         <v>32.5</v>
@@ -3721,7 +3562,7 @@
         <v>19</v>
       </c>
       <c r="B151" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C151">
         <v>32.6</v>
@@ -3735,13 +3576,13 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B152" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C152" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D152">
         <v>23.5</v>
@@ -3752,13 +3593,13 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B153" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C153" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D153">
         <v>23.5</v>
@@ -3769,13 +3610,13 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B154" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C154" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D154">
         <v>23.5</v>
@@ -3786,13 +3627,13 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B155" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C155" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D155">
         <v>24</v>
@@ -3803,13 +3644,13 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B156" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C156" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D156">
         <v>24</v>
@@ -3820,13 +3661,13 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B157" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C157" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D157">
         <v>24</v>
@@ -3837,13 +3678,13 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B158" t="s">
+        <v>114</v>
+      </c>
+      <c r="C158" t="s">
         <v>119</v>
-      </c>
-      <c r="C158" t="s">
-        <v>124</v>
       </c>
       <c r="D158">
         <v>24</v>
@@ -3854,13 +3695,13 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B159" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C159" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D159">
         <v>24</v>
@@ -3871,10 +3712,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B160" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C160">
         <v>23.5</v>
@@ -3888,10 +3729,10 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B161" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C161">
         <v>23.5</v>
@@ -3905,10 +3746,10 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B162" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C162">
         <v>23.5</v>
@@ -3922,10 +3763,10 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B163" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C163">
         <v>24</v>
@@ -3939,10 +3780,10 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B164" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C164">
         <v>24</v>
@@ -3956,10 +3797,10 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B165" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C165">
         <v>24</v>
@@ -3973,10 +3814,10 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B166" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C166">
         <v>24</v>
@@ -3990,18 +3831,1378 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
+        <v>110</v>
+      </c>
+      <c r="B167" t="s">
+        <v>120</v>
+      </c>
+      <c r="C167">
+        <v>24</v>
+      </c>
+      <c r="D167">
+        <v>24.5</v>
+      </c>
+      <c r="E167">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>110</v>
+      </c>
+      <c r="B168" t="s">
+        <v>112</v>
+      </c>
+      <c r="C168">
+        <v>23.5</v>
+      </c>
+      <c r="D168">
+        <v>23.75</v>
+      </c>
+      <c r="E168">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>110</v>
+      </c>
+      <c r="B169" t="s">
+        <v>113</v>
+      </c>
+      <c r="C169">
+        <v>23.5</v>
+      </c>
+      <c r="D169">
+        <v>23.75</v>
+      </c>
+      <c r="E169">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>110</v>
+      </c>
+      <c r="B170" t="s">
+        <v>115</v>
+      </c>
+      <c r="C170">
+        <v>23.5</v>
+      </c>
+      <c r="D170">
+        <v>23.25</v>
+      </c>
+      <c r="E170">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>110</v>
+      </c>
+      <c r="B171" t="s">
+        <v>116</v>
+      </c>
+      <c r="C171">
+        <v>24</v>
+      </c>
+      <c r="D171">
+        <v>24.5</v>
+      </c>
+      <c r="E171">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>110</v>
+      </c>
+      <c r="B172" t="s">
+        <v>117</v>
+      </c>
+      <c r="C172">
+        <v>24</v>
+      </c>
+      <c r="D172">
+        <v>24.5</v>
+      </c>
+      <c r="E172">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>110</v>
+      </c>
+      <c r="B173" t="s">
+        <v>118</v>
+      </c>
+      <c r="C173">
+        <v>24</v>
+      </c>
+      <c r="D173">
+        <v>24.5</v>
+      </c>
+      <c r="E173">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>110</v>
+      </c>
+      <c r="B174" t="s">
+        <v>119</v>
+      </c>
+      <c r="C174">
+        <v>24</v>
+      </c>
+      <c r="D174">
+        <v>24.5</v>
+      </c>
+      <c r="E174">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>110</v>
+      </c>
+      <c r="B175" t="s">
+        <v>120</v>
+      </c>
+      <c r="C175">
+        <v>24</v>
+      </c>
+      <c r="D175">
+        <v>24.5</v>
+      </c>
+      <c r="E175">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>110</v>
+      </c>
+      <c r="B176" t="s">
+        <v>112</v>
+      </c>
+      <c r="C176">
+        <v>23.5</v>
+      </c>
+      <c r="D176">
+        <v>23.75</v>
+      </c>
+      <c r="E176">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>110</v>
+      </c>
+      <c r="B177" t="s">
+        <v>113</v>
+      </c>
+      <c r="C177">
+        <v>23.5</v>
+      </c>
+      <c r="D177">
+        <v>23.75</v>
+      </c>
+      <c r="E177">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>110</v>
+      </c>
+      <c r="B178" t="s">
+        <v>115</v>
+      </c>
+      <c r="C178">
+        <v>23.5</v>
+      </c>
+      <c r="D178">
+        <v>23.25</v>
+      </c>
+      <c r="E178">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>110</v>
+      </c>
+      <c r="B179" t="s">
+        <v>116</v>
+      </c>
+      <c r="C179">
+        <v>24</v>
+      </c>
+      <c r="D179">
+        <v>24.5</v>
+      </c>
+      <c r="E179">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>110</v>
+      </c>
+      <c r="B180" t="s">
+        <v>117</v>
+      </c>
+      <c r="C180">
+        <v>24</v>
+      </c>
+      <c r="D180">
+        <v>24.5</v>
+      </c>
+      <c r="E180">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>110</v>
+      </c>
+      <c r="B181" t="s">
+        <v>118</v>
+      </c>
+      <c r="C181">
+        <v>24</v>
+      </c>
+      <c r="D181">
+        <v>24.5</v>
+      </c>
+      <c r="E181">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>110</v>
+      </c>
+      <c r="B182" t="s">
+        <v>119</v>
+      </c>
+      <c r="C182">
+        <v>24</v>
+      </c>
+      <c r="D182">
+        <v>24.5</v>
+      </c>
+      <c r="E182">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>110</v>
+      </c>
+      <c r="B183" t="s">
+        <v>120</v>
+      </c>
+      <c r="C183">
+        <v>24</v>
+      </c>
+      <c r="D183">
+        <v>24.5</v>
+      </c>
+      <c r="E183">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>110</v>
+      </c>
+      <c r="B184" t="s">
+        <v>112</v>
+      </c>
+      <c r="C184">
+        <v>23.5</v>
+      </c>
+      <c r="D184">
+        <v>23.75</v>
+      </c>
+      <c r="E184">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>110</v>
+      </c>
+      <c r="B185" t="s">
+        <v>113</v>
+      </c>
+      <c r="C185">
+        <v>23.5</v>
+      </c>
+      <c r="D185">
+        <v>23.75</v>
+      </c>
+      <c r="E185">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>110</v>
+      </c>
+      <c r="B186" t="s">
+        <v>115</v>
+      </c>
+      <c r="C186">
+        <v>23.5</v>
+      </c>
+      <c r="D186">
+        <v>23.25</v>
+      </c>
+      <c r="E186">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>110</v>
+      </c>
+      <c r="B187" t="s">
+        <v>116</v>
+      </c>
+      <c r="C187">
+        <v>24</v>
+      </c>
+      <c r="D187">
+        <v>24.5</v>
+      </c>
+      <c r="E187">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>110</v>
+      </c>
+      <c r="B188" t="s">
+        <v>117</v>
+      </c>
+      <c r="C188">
+        <v>24</v>
+      </c>
+      <c r="D188">
+        <v>24.5</v>
+      </c>
+      <c r="E188">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>110</v>
+      </c>
+      <c r="B189" t="s">
+        <v>118</v>
+      </c>
+      <c r="C189">
+        <v>24</v>
+      </c>
+      <c r="D189">
+        <v>24.5</v>
+      </c>
+      <c r="E189">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>110</v>
+      </c>
+      <c r="B190" t="s">
+        <v>119</v>
+      </c>
+      <c r="C190">
+        <v>24</v>
+      </c>
+      <c r="D190">
+        <v>24.5</v>
+      </c>
+      <c r="E190">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>110</v>
+      </c>
+      <c r="B191" t="s">
+        <v>120</v>
+      </c>
+      <c r="C191">
+        <v>24</v>
+      </c>
+      <c r="D191">
+        <v>24.5</v>
+      </c>
+      <c r="E191">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>110</v>
+      </c>
+      <c r="B192" t="s">
+        <v>112</v>
+      </c>
+      <c r="C192">
+        <v>23.5</v>
+      </c>
+      <c r="D192">
+        <v>23.75</v>
+      </c>
+      <c r="E192">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>110</v>
+      </c>
+      <c r="B193" t="s">
+        <v>113</v>
+      </c>
+      <c r="C193">
+        <v>23.5</v>
+      </c>
+      <c r="D193">
+        <v>23.75</v>
+      </c>
+      <c r="E193">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>110</v>
+      </c>
+      <c r="B194" t="s">
+        <v>115</v>
+      </c>
+      <c r="C194">
+        <v>23.5</v>
+      </c>
+      <c r="D194">
+        <v>23.25</v>
+      </c>
+      <c r="E194">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>110</v>
+      </c>
+      <c r="B195" t="s">
+        <v>116</v>
+      </c>
+      <c r="C195">
+        <v>24</v>
+      </c>
+      <c r="D195">
+        <v>24.5</v>
+      </c>
+      <c r="E195">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>110</v>
+      </c>
+      <c r="B196" t="s">
+        <v>117</v>
+      </c>
+      <c r="C196">
+        <v>24</v>
+      </c>
+      <c r="D196">
+        <v>24.5</v>
+      </c>
+      <c r="E196">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>110</v>
+      </c>
+      <c r="B197" t="s">
+        <v>118</v>
+      </c>
+      <c r="C197">
+        <v>24</v>
+      </c>
+      <c r="D197">
+        <v>24.5</v>
+      </c>
+      <c r="E197">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>110</v>
+      </c>
+      <c r="B198" t="s">
+        <v>119</v>
+      </c>
+      <c r="C198">
+        <v>24</v>
+      </c>
+      <c r="D198">
+        <v>24.5</v>
+      </c>
+      <c r="E198">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>110</v>
+      </c>
+      <c r="B199" t="s">
+        <v>120</v>
+      </c>
+      <c r="C199">
+        <v>24</v>
+      </c>
+      <c r="D199">
+        <v>24.5</v>
+      </c>
+      <c r="E199">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>110</v>
+      </c>
+      <c r="B200" t="s">
+        <v>112</v>
+      </c>
+      <c r="C200">
+        <v>23.5</v>
+      </c>
+      <c r="D200">
+        <v>23.75</v>
+      </c>
+      <c r="E200">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>110</v>
+      </c>
+      <c r="B201" t="s">
+        <v>113</v>
+      </c>
+      <c r="C201">
+        <v>23.5</v>
+      </c>
+      <c r="D201">
+        <v>23.75</v>
+      </c>
+      <c r="E201">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>110</v>
+      </c>
+      <c r="B202" t="s">
+        <v>115</v>
+      </c>
+      <c r="C202">
+        <v>23.5</v>
+      </c>
+      <c r="D202">
+        <v>23.25</v>
+      </c>
+      <c r="E202">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>110</v>
+      </c>
+      <c r="B203" t="s">
+        <v>116</v>
+      </c>
+      <c r="C203">
+        <v>24</v>
+      </c>
+      <c r="D203">
+        <v>24.5</v>
+      </c>
+      <c r="E203">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>110</v>
+      </c>
+      <c r="B204" t="s">
+        <v>117</v>
+      </c>
+      <c r="C204">
+        <v>24</v>
+      </c>
+      <c r="D204">
+        <v>24.5</v>
+      </c>
+      <c r="E204">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>110</v>
+      </c>
+      <c r="B205" t="s">
+        <v>118</v>
+      </c>
+      <c r="C205">
+        <v>24</v>
+      </c>
+      <c r="D205">
+        <v>24.5</v>
+      </c>
+      <c r="E205">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>110</v>
+      </c>
+      <c r="B206" t="s">
+        <v>119</v>
+      </c>
+      <c r="C206">
+        <v>24</v>
+      </c>
+      <c r="D206">
+        <v>24.5</v>
+      </c>
+      <c r="E206">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>110</v>
+      </c>
+      <c r="B207" t="s">
+        <v>120</v>
+      </c>
+      <c r="C207">
+        <v>24</v>
+      </c>
+      <c r="D207">
+        <v>24.5</v>
+      </c>
+      <c r="E207">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>110</v>
+      </c>
+      <c r="B208" t="s">
+        <v>112</v>
+      </c>
+      <c r="C208">
+        <v>23.5</v>
+      </c>
+      <c r="D208">
+        <v>23.75</v>
+      </c>
+      <c r="E208">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>110</v>
+      </c>
+      <c r="B209" t="s">
+        <v>113</v>
+      </c>
+      <c r="C209">
+        <v>23.5</v>
+      </c>
+      <c r="D209">
+        <v>23.75</v>
+      </c>
+      <c r="E209">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>110</v>
+      </c>
+      <c r="B210" t="s">
+        <v>115</v>
+      </c>
+      <c r="C210">
+        <v>23.5</v>
+      </c>
+      <c r="D210">
+        <v>23.25</v>
+      </c>
+      <c r="E210">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>110</v>
+      </c>
+      <c r="B211" t="s">
+        <v>116</v>
+      </c>
+      <c r="C211">
+        <v>24</v>
+      </c>
+      <c r="D211">
+        <v>24.5</v>
+      </c>
+      <c r="E211">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>110</v>
+      </c>
+      <c r="B212" t="s">
+        <v>117</v>
+      </c>
+      <c r="C212">
+        <v>24</v>
+      </c>
+      <c r="D212">
+        <v>24.5</v>
+      </c>
+      <c r="E212">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>110</v>
+      </c>
+      <c r="B213" t="s">
+        <v>118</v>
+      </c>
+      <c r="C213">
+        <v>24</v>
+      </c>
+      <c r="D213">
+        <v>24.5</v>
+      </c>
+      <c r="E213">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>110</v>
+      </c>
+      <c r="B214" t="s">
+        <v>119</v>
+      </c>
+      <c r="C214">
+        <v>24</v>
+      </c>
+      <c r="D214">
+        <v>24.5</v>
+      </c>
+      <c r="E214">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>110</v>
+      </c>
+      <c r="B215" t="s">
+        <v>120</v>
+      </c>
+      <c r="C215">
+        <v>24</v>
+      </c>
+      <c r="D215">
+        <v>24.5</v>
+      </c>
+      <c r="E215">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>110</v>
+      </c>
+      <c r="B216" t="s">
+        <v>112</v>
+      </c>
+      <c r="C216">
+        <v>23.5</v>
+      </c>
+      <c r="D216">
+        <v>23.75</v>
+      </c>
+      <c r="E216">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>110</v>
+      </c>
+      <c r="B217" t="s">
+        <v>113</v>
+      </c>
+      <c r="C217">
+        <v>23.5</v>
+      </c>
+      <c r="D217">
+        <v>23.75</v>
+      </c>
+      <c r="E217">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>110</v>
+      </c>
+      <c r="B218" t="s">
+        <v>115</v>
+      </c>
+      <c r="C218">
+        <v>23.5</v>
+      </c>
+      <c r="D218">
+        <v>23.25</v>
+      </c>
+      <c r="E218">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>110</v>
+      </c>
+      <c r="B219" t="s">
+        <v>116</v>
+      </c>
+      <c r="C219">
+        <v>24</v>
+      </c>
+      <c r="D219">
+        <v>24.5</v>
+      </c>
+      <c r="E219">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>110</v>
+      </c>
+      <c r="B220" t="s">
+        <v>117</v>
+      </c>
+      <c r="C220">
+        <v>24</v>
+      </c>
+      <c r="D220">
+        <v>24.5</v>
+      </c>
+      <c r="E220">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>110</v>
+      </c>
+      <c r="B221" t="s">
+        <v>118</v>
+      </c>
+      <c r="C221">
+        <v>24</v>
+      </c>
+      <c r="D221">
+        <v>24.5</v>
+      </c>
+      <c r="E221">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>110</v>
+      </c>
+      <c r="B222" t="s">
+        <v>119</v>
+      </c>
+      <c r="C222">
+        <v>24</v>
+      </c>
+      <c r="D222">
+        <v>24.5</v>
+      </c>
+      <c r="E222">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>110</v>
+      </c>
+      <c r="B223" t="s">
+        <v>120</v>
+      </c>
+      <c r="C223">
+        <v>24</v>
+      </c>
+      <c r="D223">
+        <v>24.5</v>
+      </c>
+      <c r="E223">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
         <v>20</v>
       </c>
-      <c r="B167" t="s">
-        <v>125</v>
-      </c>
-      <c r="C167">
-        <v>24</v>
-      </c>
-      <c r="D167">
-        <v>24.5</v>
-      </c>
-      <c r="E167">
+      <c r="B224" t="s">
+        <v>112</v>
+      </c>
+      <c r="C224">
+        <v>23.5</v>
+      </c>
+      <c r="D224">
+        <v>23.75</v>
+      </c>
+      <c r="E224">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>20</v>
+      </c>
+      <c r="B225" t="s">
+        <v>113</v>
+      </c>
+      <c r="C225">
+        <v>23.5</v>
+      </c>
+      <c r="D225">
+        <v>23.75</v>
+      </c>
+      <c r="E225">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>20</v>
+      </c>
+      <c r="B226" t="s">
+        <v>115</v>
+      </c>
+      <c r="C226">
+        <v>23.5</v>
+      </c>
+      <c r="D226">
+        <v>23.25</v>
+      </c>
+      <c r="E226">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>20</v>
+      </c>
+      <c r="B227" t="s">
+        <v>116</v>
+      </c>
+      <c r="C227">
+        <v>24</v>
+      </c>
+      <c r="D227">
+        <v>24.5</v>
+      </c>
+      <c r="E227">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>20</v>
+      </c>
+      <c r="B228" t="s">
+        <v>117</v>
+      </c>
+      <c r="C228">
+        <v>24</v>
+      </c>
+      <c r="D228">
+        <v>24.5</v>
+      </c>
+      <c r="E228">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>20</v>
+      </c>
+      <c r="B229" t="s">
+        <v>118</v>
+      </c>
+      <c r="C229">
+        <v>24</v>
+      </c>
+      <c r="D229">
+        <v>24.5</v>
+      </c>
+      <c r="E229">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>20</v>
+      </c>
+      <c r="B230" t="s">
+        <v>119</v>
+      </c>
+      <c r="C230">
+        <v>24</v>
+      </c>
+      <c r="D230">
+        <v>24.5</v>
+      </c>
+      <c r="E230">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>20</v>
+      </c>
+      <c r="B231" t="s">
+        <v>120</v>
+      </c>
+      <c r="C231">
+        <v>24</v>
+      </c>
+      <c r="D231">
+        <v>24.5</v>
+      </c>
+      <c r="E231">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>20</v>
+      </c>
+      <c r="B232" t="s">
+        <v>112</v>
+      </c>
+      <c r="C232">
+        <v>23.5</v>
+      </c>
+      <c r="D232">
+        <v>23.75</v>
+      </c>
+      <c r="E232">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>20</v>
+      </c>
+      <c r="B233" t="s">
+        <v>113</v>
+      </c>
+      <c r="C233">
+        <v>23.5</v>
+      </c>
+      <c r="D233">
+        <v>23.75</v>
+      </c>
+      <c r="E233">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>20</v>
+      </c>
+      <c r="B234" t="s">
+        <v>115</v>
+      </c>
+      <c r="C234">
+        <v>23.5</v>
+      </c>
+      <c r="D234">
+        <v>23.25</v>
+      </c>
+      <c r="E234">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
+        <v>20</v>
+      </c>
+      <c r="B235" t="s">
+        <v>116</v>
+      </c>
+      <c r="C235">
+        <v>24</v>
+      </c>
+      <c r="D235">
+        <v>24.5</v>
+      </c>
+      <c r="E235">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>20</v>
+      </c>
+      <c r="B236" t="s">
+        <v>117</v>
+      </c>
+      <c r="C236">
+        <v>24</v>
+      </c>
+      <c r="D236">
+        <v>24.5</v>
+      </c>
+      <c r="E236">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>20</v>
+      </c>
+      <c r="B237" t="s">
+        <v>118</v>
+      </c>
+      <c r="C237">
+        <v>24</v>
+      </c>
+      <c r="D237">
+        <v>24.5</v>
+      </c>
+      <c r="E237">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
+        <v>20</v>
+      </c>
+      <c r="B238" t="s">
+        <v>119</v>
+      </c>
+      <c r="C238">
+        <v>24</v>
+      </c>
+      <c r="D238">
+        <v>24.5</v>
+      </c>
+      <c r="E238">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
+        <v>20</v>
+      </c>
+      <c r="B239" t="s">
+        <v>120</v>
+      </c>
+      <c r="C239">
+        <v>24</v>
+      </c>
+      <c r="D239">
+        <v>24.5</v>
+      </c>
+      <c r="E239">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
+        <v>20</v>
+      </c>
+      <c r="B240" t="s">
+        <v>112</v>
+      </c>
+      <c r="C240">
+        <v>23.5</v>
+      </c>
+      <c r="D240">
+        <v>23.75</v>
+      </c>
+      <c r="E240">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>20</v>
+      </c>
+      <c r="B241" t="s">
+        <v>113</v>
+      </c>
+      <c r="C241">
+        <v>23.5</v>
+      </c>
+      <c r="D241">
+        <v>23.75</v>
+      </c>
+      <c r="E241">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A242" t="s">
+        <v>20</v>
+      </c>
+      <c r="B242" t="s">
+        <v>115</v>
+      </c>
+      <c r="C242">
+        <v>23.5</v>
+      </c>
+      <c r="D242">
+        <v>23.25</v>
+      </c>
+      <c r="E242">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A243" t="s">
+        <v>20</v>
+      </c>
+      <c r="B243" t="s">
+        <v>116</v>
+      </c>
+      <c r="C243">
+        <v>24</v>
+      </c>
+      <c r="D243">
+        <v>24.5</v>
+      </c>
+      <c r="E243">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A244" t="s">
+        <v>20</v>
+      </c>
+      <c r="B244" t="s">
+        <v>117</v>
+      </c>
+      <c r="C244">
+        <v>24</v>
+      </c>
+      <c r="D244">
+        <v>24.5</v>
+      </c>
+      <c r="E244">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A245" t="s">
+        <v>20</v>
+      </c>
+      <c r="B245" t="s">
+        <v>118</v>
+      </c>
+      <c r="C245">
+        <v>24</v>
+      </c>
+      <c r="D245">
+        <v>24.5</v>
+      </c>
+      <c r="E245">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>20</v>
+      </c>
+      <c r="B246" t="s">
+        <v>119</v>
+      </c>
+      <c r="C246">
+        <v>24</v>
+      </c>
+      <c r="D246">
+        <v>24.5</v>
+      </c>
+      <c r="E246">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>20</v>
+      </c>
+      <c r="B247" t="s">
+        <v>120</v>
+      </c>
+      <c r="C247">
+        <v>24</v>
+      </c>
+      <c r="D247">
+        <v>24.5</v>
+      </c>
+      <c r="E247">
         <v>85</v>
       </c>
     </row>

</xml_diff>